<commit_message>
Refactor main file, excel output complete
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Price</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -368,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -380,33 +383,36 @@
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>2</v>
       </c>

</xml_diff>